<commit_message>
update readme and data scopus
</commit_message>
<xml_diff>
--- a/analisis.xlsx
+++ b/analisis.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="83">
   <si>
     <t>OUTPUT NARASI</t>
   </si>
@@ -71,168 +71,206 @@
     <t>Tidak Tersitasi</t>
   </si>
   <si>
-    <t>Mungkin Tidak</t>
-  </si>
-  <si>
-    <t>[1] S. Zhang, X. Li, M. Zong, X. Zhu, and D. Cheng, “Learning k for kNN Classification,” ACM Trans. Intell. Syst. Technol., vol. 8, no. 3, 2017, doi: 10.1145/2990508.</t>
-  </si>
-  <si>
-    <t>[2] X. Wu et al., Top 10 algorithms in data mining, vol. 14, no. 1. 2008.</t>
-  </si>
-  <si>
-    <t>[3] N. O’Mahony et al., “Deep Learning vs. Traditional Computer Vision,” Adv. Intell. Syst. Comput., vol. 943, no. Cv, pp. 128–144, 2020, doi: 10.1007/978-3-030-17795-9_10.</t>
-  </si>
-  <si>
-    <t>[4] K. O’Shea and R. Nash, “An Introduction to Convolutional Neural Networks,” pp. 1–11, 2015, [Online]. Available: http://arxiv.org/abs/1511.08458.</t>
-  </si>
-  <si>
-    <t>[5] A. A. M. Al-Saffar, H. Tao, and M. A. Talab, “Review of deep convolution neural network in image classification,” Proceeding - 2017 Int. Conf. Radar, Antenna, Microwave, Electron. Telecommun. ICRAMET 2017, vol. 2018-Janua, pp. 26–31, 2017, doi: 10.1109/ICRAMET.2017.8253139.</t>
-  </si>
-  <si>
-    <t>[6] M. Pak and S. Kim, “A review of deep learning in image recognition,” Proc. 2017 4th Int. Conf. Comput. Appl. Inf. Process. Technol. CAIPT 2017, vol. 2018-Janua, pp. 1–3, 2018, doi: 10.1109/CAIPT.2017.8320684.</t>
-  </si>
-  <si>
-    <t>[7] E. Setiawan and A. Muttaqin, “Implementation of K-Nearest Neighbors face recognition on low-power processor,” Telkomnika (Telecommunication Comput. Electron. Control., vol. 13, no. 3, pp. 949–954, 2015, doi: 10.12928/telkomnika.v13i3.713.</t>
-  </si>
-  <si>
-    <t>[8] P. M. Shah, “Face detection from images using support vector machine,” 2012.</t>
-  </si>
-  <si>
-    <t>[9] M. T. Ghazal and K. Abdullah, “Face recognition based on curvelets, invariant moments features and SVM,” Telkomnika (Telecommunication Comput. Electron. Control., vol. 18, no. 2, pp. 733–739, 2020, doi: 10.12928/TELKOMNIKA.v18i2.14106.</t>
-  </si>
-  <si>
-    <t>[10] A. R. Syafeeza, M. Khalil-Hani, S. S. Liew, and R. Bakhteri, “Convolutional neural network for face recognition with pose and illumination variation,” Int. J. Eng. Technol., vol. 6, no. 1, pp. 44–57, 2014.</t>
-  </si>
-  <si>
-    <t>[11] C. Jagadeeswari and M. U. Theja, “Performance Evaluation of Intelligent Face Mask Detection System with various Deep Learning Classifiers Keywords :,” Int. J. Adv. Sci. Technol., vol. 29, no. 11, pp. 3074–3082, 2020.</t>
-  </si>
-  <si>
-    <t>[12] W. Han, Z. Huang, A. Kuerban, M. Yan, and H. Fu, “A Mask Detection Method for Shoppers under the Threat of COVID-19 Coronavirus,” in Proceedings - 2020 International Conference on Computer Vision, Image and Deep Learning, CVIDL 2020, Jul. 2020, pp. 442–447, doi: 10.1109/CVIDL51233.2020.00-54.</t>
-  </si>
-  <si>
-    <t>[13] V. Vinitha and V. Velantina, “Covid-19 Facemask Detection With Deep Learning and Computer Vision,” Int. Res. J. Eng. Technol., vol. 7, no. 8, pp. 3127–3132, 2020.</t>
-  </si>
-  <si>
-    <t>[14] P. Nagrath, R. Jain, A. Madan, R. Arora, P. Kataria, and J. Hemanth, “SSDMNV2: A real time DNN-based face mask detection system using single shot multibox detector and MobileNetV2,” Sustain. Cities Soc., vol. 66, no. December 2020, 2021, doi: 10.1016/j.scs.2020.102692.</t>
-  </si>
-  <si>
-    <t>[15] S. Ge, J. Li, Q. Ye, and Z. Luo, “Detecting masked faces in the wild with LLE-CNNs,” Proc. - 30th IEEE Conf. Comput. Vis. Pattern Recognition, CVPR 2017, vol. 2017-Janua, pp. 426–434, 2017, doi: 10.1109/CVPR.2017.53.</t>
-  </si>
-  <si>
-    <t>[16] M. Grassi and M. Faundez-Zanuy, “Face recognition with facial mask application and neural networks,” Lect. Notes Comput. Sci. (including Subser. Lect. Notes Artif. Intell. Lect. Notes Bioinformatics), vol. 4507 LNCS, pp. 709–716, 2007, doi: 10.1007/978-3-54073007-1_85.</t>
-  </si>
-  <si>
-    <t>[17] A. Shustanov and P. Yakimov, “CNN Design for Real-Time Traffic Sign Recognition,” Procedia Eng., vol. 201, pp. 718–725, 2017, doi: 10.1016/j.proeng.2017.09.594.</t>
-  </si>
-  <si>
-    <t>[18] Larxel, “Face Mask Detection | Kaggle,” 2020. https://www.kaggle.com/omkargurav/face-mask-dataset (accessed Feb. 01, 2021).</t>
-  </si>
-  <si>
-    <t>[19] F. Chollet and &amp; O., “Keras: the Python deep learning API,” Keras: the Python deep learning API, 2020. https://keras.io/ (accessed Dec. 18, 2020).</t>
-  </si>
-  <si>
-    <t>[20] T. F. Gonzalez, “Handbook of approximation algorithms and metaheuristics,” Handb. Approx. Algorithms Metaheuristics, pp. 1–1432, 2007, doi: 10.1201/9781420010749.</t>
-  </si>
-  <si>
-    <t>[21] C. Szegedy et al., “Going deeper with convolutions,” Proc. IEEE Comput. Soc. Conf. Comput. Vis. Pattern Recognit., vol. 07-12-June, pp. 1–9, 2015, doi: 10.1109/CVPR.2015.7298594.</t>
-  </si>
-  <si>
-    <t>[22] K. Simonyan and A. Zisserman, “Very deep convolutional networks for large-scale image recognition,” 3rd Int. Conf. Learn. Represent. ICLR 2015 - Conf. Track Proc., pp. 1–14, 2015.</t>
-  </si>
-  <si>
-    <t>[23] M. D. Zeiler and R. Fergus, “Visualizing and understanding convolutional networks,” Lect. Notes Comput. Sci. (including Subser. Lect. Notes Artif. Intell. Lect. Notes Bioinformatics), vol. 8689 LNCS, no. PART 1, pp. 818–833, 2014, doi: 10.1007/978-3-319-10590-1_53.</t>
-  </si>
-  <si>
-    <t>[24] K. He, X. Zhang, S. Ren, and J. Sun, “Deep residual learning for image recognition,” Proc. IEEE Comput. Soc. Conf. Comput. Vis. Pattern Recognit., vol. 2016-Decem, pp. 770–778, 2016, doi: 10.1109/CVPR.2016.90.</t>
+    <t>Tidak</t>
+  </si>
+  <si>
+    <t>[1] Soehodho Sutanto, “Public Transportation Development and Traffic Accident Prevention in Indonesia,” IATSS Research, vol. 38, no. 1, pp. 7–13, Jul. 2014, doi: 10.1016/j.iatssr.2014.06.001.</t>
+  </si>
+  <si>
+    <t>[2] R. D. Kusumastuti, Viverita, Z. A. Husodo, L. Suardi, and D. N. Danarsari, “Developing a resilience index towards natural disasters in Indonesia,” International Journal of Disaster Risk Reduction, vol. 10, no. PA, pp. 327–340, Dec. 2014, doi: 10.1016/j.ijdrr.2014.10.007.</t>
+  </si>
+  <si>
+    <t>[3] T.-H. Chen, P.-H. Wu, and Y.-C. Chiou, “An Early Fire-Detection Method Based on Image Processing,” in International Conference on Image Processing, 2004, pp. 1707–1710.</t>
+  </si>
+  <si>
+    <t>[4] K. Muhammad, J. Ahmad, and S. W. Baik, “Early fire detection using convolutional neural networks during surveillance for effective disaster management,” Neurocomputing, vol. 288, pp. 30–42, May 2018, doi: 10.1016/j.neucom.2017.04.083.</t>
+  </si>
+  <si>
+    <t>[5] S. Dabiri and K. Heaslip, “Developing a Twitter-based traffic event detection model using deep learning architectures,” Expert Systems with Applications, vol. 118, pp. 425–439, Mar. 2019, doi: 10.1016/j.eswa.2018.10.017.</t>
+  </si>
+  <si>
+    <t>[6] F. Ali, A. Ali, M. Imran, R. A. Naqvi, M. H. Siddiqi, and K. S. Kwak, “Traffic accident detection and condition analysis based on social networking data,” Accident Analysis and Prevention, vol. 151, Mar. 2021, doi: 10.1016/j.aap.2021.105973.</t>
+  </si>
+  <si>
+    <t>[7] S. Dabiri, K. Heaslip, and C. E. Via, “Transport-domain applications of widely used data sources in the smart transportation: A survey,” arXiv preprint 1803.10902. 2018.</t>
+  </si>
+  <si>
+    <t>[8] H. Abu-Gellban, “A Survey of Real-Time Social-Based Traffic Detection,” in International Conference on Intelligence and Security Informatics, Nov. 2020, pp. 1–6. doi: 10.1109/ISI49825.2020.9280534.</t>
+  </si>
+  <si>
+    <t>[9] A. N. Rasyid and A. Purwarianti, “Sentiment Classification for Indonesian Message in Social Media,” in International Conference on Cloud Computing and Social Networking (ICCCSN), 2012, pp. 1–5. doi: 10.1109/ICCCSN.2012.6215730.</t>
+  </si>
+  <si>
+    <t>[10] M Lailiyah, S Sumpeno, and I.K.E Purnama, “Sentiment Analysis of Public Complaints Using Lexical Resources Between Indonesian Sentiment Lexicon and Sentiwordnet,” in International Seminar on Intelligent Technology and Its Application, 2017, pp. 307–312. doi: 10.1109/ISITIA.2017.8124100.</t>
+  </si>
+  <si>
+    <t>[11] F. N. Putra and C. Fatichah, “Klasifikasi jenis kejadian menggunakan kombinasi neuroner dan recurrent convolutional neural network pada data twitter,” Register: Jurnal Ilmiah Teknologi Sistem Informasi, vol. 4, no. 2, pp. 81–90, Jul. 2018, doi: 10.26594/register.v4i2.1242.</t>
+  </si>
+  <si>
+    <t>[12] S. Dabiri and K. Heaslip, “Developing a Twitter-based traffic event detection model using deep learning architectures,” Expert Systems with Applications, vol. 118, pp. 425–439, Mar. 2019, doi: 10.1016/j.eswa.2018.10.017.</t>
+  </si>
+  <si>
+    <t>[13] R. Hendrawan and S. al Faraby, “Multilabel Classification of Hate Speech and Abusive Words on Indonesian Twitter Social Media,” in 2020 International Conference on Data Science and Its Applications, 2020, pp. 1–7.</t>
+  </si>
+  <si>
+    <t>[14] M. O. Ibrohim and I. Budi, “Multi-label Hate Speech and Abusive Language Detection in Indonesian Twitter,” in Proceedings of the Third Workshop on Abusive Language Online, 2019, pp. 46–57. doi: https://doi.org/10.18653/v1/W19-3506.</t>
+  </si>
+  <si>
+    <t>[15] A. Omar, T. M. Mahmoud, T. Abd-El-Hafeez, and A. Mahfouz, “Multi-label Arabic text classification in Online Social Networks,” Information Systems, vol. 100, Sep. 2021, doi: 10.1016/j.is.2021.101785.</t>
+  </si>
+  <si>
+    <t>[16] M. A. Parwez, M. Abulaish, and Jahiruddin, “Multi-Label Classification of Microblogging Texts Using Convolution Neural Network,” IEEE Access, vol. 7, pp. 68678–68691, 2019, doi: 10.1109/ACCESS.2019.2919494.</t>
+  </si>
+  <si>
+    <t>[17] P. Mercader and J. Haddad, “Automatic incident detection on freeways based on Bluetooth traffic monitoring,” Accident Analysis and Prevention, vol. 146, Oct. 2020, doi: 10.1016/j.aap.2020.105703.</t>
+  </si>
+  <si>
+    <t>[18] Z. Zheng, C. Wang, P. Wang, Y. Xiong, F. Zhang, and Y. Lv, “Framework for fusing traffic information from social and physical transportation data,” PLoS ONE, vol. 13, no. 8, Aug. 2018, doi: 10.1371/journal.pone.0201531. Last Name Author1, Last Name Author2, &amp; Last Name Author3 Journal of Information Systems Engineering and Business Intelligence, XXXX, X (X), pp-pp</t>
+  </si>
+  <si>
+    <t>[19] S. Wang et al., “Computing urban traffic congestions by incorporating sparse GPS probe data and social media data,” ACM Transactions on Information Systems, vol. 35, no. 4, Jul. 2017, doi: 10.1145/3057281.</t>
+  </si>
+  <si>
+    <t>[20] Y. Gu, Z. Qian, and F. Chen, “From Twitter to detector: Real-time traffic incident detection using social media data,” Transportation Research Part C: Emerging Technologies, vol. 67, pp. 321–342, Jun. 2016, doi: 10.1016/j.trc.2016.02.011.</t>
+  </si>
+  <si>
+    <t>[21] Dwi Lingga P Rendra, Fatichah Chastine, and Purwitasari Diana, “Deteksi Gempa Berdasarkan Data Twitter Menggunakan Decision Tree, Random Forest, dan SVM,” JURNAL TEKNIK ITS, vol. 6, no. 1, pp. 159–162, 2017.</t>
+  </si>
+  <si>
+    <t>[22] D. Tang, B. Qin, and T. Liu, “Document Modeling with Gated Recurrent Neural Network for Sentiment Classification,” in Empirical Methods in Natural Language Processing, 2015, pp. 1422– 1432. doi: 10.18653/v1/D15-1167.</t>
+  </si>
+  <si>
+    <t>[23] Y. Kim, “Convolutional Neural Networks for Sentence Classification,” in Empirical Methods in Natural Language Processing, Oct. 2014, pp. 1746–1751. doi: https://doi.org/10.3115/v1/D14-1181.</t>
+  </si>
+  <si>
+    <t>[24] W. Liao, Y. Wang, Y. Yin, X. Zhang, and P. Ma, “Improved sequence generation model for multilabel classification via CNN and initialized fully connection,” Neurocomputing, vol. 382, pp. 188– 195, Mar. 2020, doi: 10.1016/j.neucom.2019.11.074.</t>
+  </si>
+  <si>
+    <t>[25] H. Peng et al., “Hierarchical Taxonomy-Aware and Attentional Graph Capsule RCNNs for LargeScale Multi-Label Text Classification,” IEEE Transactions on Knowledge and Data Engineering, vol. 33, no. 6, pp. 2505–2519, Jun. 2021, doi: 10.1109/TKDE.2019.2959991.</t>
+  </si>
+  <si>
+    <t>[26] S. Lai, L. Xu, K. Liu, and J. Zhao, “Recurrent Convolutional Neural Networks for Text Classification,” in Twenty-Ninth AAAI Conference on Artificial Intelligence2267, 2015, pp. 2267– 2273.</t>
+  </si>
+  <si>
+    <t>[27] C. Zhou, C. Sun, Z. Liu, and F. C. M. Lau, “A C-LSTM Neural Network for Text Classification,” arXiv preprint arXiv:1511.08630. 2015.</t>
+  </si>
+  <si>
+    <t>[28] H. J. Dai, P. T. Lai, Y. C. Chang, and R. T. H. Tsai, “Enhancing of chemical compound and drug name recognition using representative tag scheme and fine-grained tokenization,” Journal of Cheminformatics, vol. 7, 2015, doi: 10.1186/1758-2946-7-S1-S14.</t>
+  </si>
+  <si>
+    <t>[29] G. Lample, M. Ballesteros, S. Subramanian, K. Kawakami, and C. Dyer, “Neural Architectures for Named Entity Recognition,” in Proceedings of NAACL-HLT, 2016, pp. 260–270.</t>
+  </si>
+  <si>
+    <t>[30] F. A. Gers, N. N. Schraudolph, and J. Schmidhuber, “Learning Precise Timing with LSTM Recurrent Networks,” Journal of Machine Learning Research, vol. 3, pp. 115–143, 2002.</t>
+  </si>
+  <si>
+    <t>[31] J. Nam, J. Kim, E. Loza Mencía, I. Gurevych, and J. Fürnkranz, “Large-Scale Multi-label Text Classification — Revisiting Neural Networks,” in Machine Learning and Knowledge Discovery in Databases, 2014, pp. 437–452. doi: https://doi.org/10.1007/978-3-662-44851-9_28.</t>
+  </si>
+  <si>
+    <t>[32] J. Wang, L. Chen, J. Zhang, Y. Yuan, M. Li, and W. H. Zeng, “CNN transfer learning for automatic image-based classification of crop disease,” in Communications in Computer and Information Science, 2018, vol. 875, pp. 319–329. doi: 10.1007/978-981-13-1702-6_32. &lt;&lt;Do Not Remove this page&gt;&gt; &lt;&lt; This checklist must fill when submitted to JISEBI&gt;&gt; Authors Submission Checklist All manuscript must meet the following criteria to be processed into the peer-review stage. Failure to meet the following criteria may increase the processing time of the manuscript or even rejection. Write OK if the authors have confirmed that the manuscript meets the criteria. If the author cannot fulfill these criteria, give a reason and write in the checklist with highlighted text. 1 Template and Layout Authors Claim &amp; Comment Editors Comment 1.1 Have used the latest JISEBI template (latest update Feb 2019) √ 1.2 Introduction, Literature Review (optional), Methods, Result,</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
   <si>
     <t>2017</t>
   </si>
   <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2020</t>
+    <t>Tidak Lengkap (*T)</t>
+  </si>
+  <si>
+    <t>Kosong</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t>2015</t>
   </si>
   <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2016</t>
+    <t>2002</t>
   </si>
   <si>
     <t>Tahun terbit</t>
   </si>
   <si>
-    <t>Referensi yang digunakan pada paper ini dianggap mutakhir sebesar 87.50%. Referensi dianggap mutakhir ketika tahun terbit referensi berumur maksimal 10 tahun pada saat sistem digunakan. 
-Referensi dengan Nomor 2 16 20 tidak mutakhir.</t>
-  </si>
-  <si>
-    <t>Tidak</t>
-  </si>
-  <si>
-    <t>Referensi yang digunakan pada paper ini terindikasi self-citation sebesar 0.00%. Sebuah referensi dianggap self-citation jika nama penulis paper dan nama author pada referensi memiliki kesamaan.</t>
-  </si>
-  <si>
-    <t>Mungkin tidak</t>
+    <t>Referensi yang digunakan pada paper ini dianggap mutakhir sebesar 90.62%. Referensi dianggap mutakhir ketika tahun terbit referensi berumur maksimal 10 tahun pada saat sistem digunakan. 
+Referensi dengan Nomor 3 14 30 tidak mutakhir.</t>
+  </si>
+  <si>
+    <t>Iya</t>
+  </si>
+  <si>
+    <t>Referensi yang digunakan pada paper ini terindikasi self-citation sebesar 3.12%. Sebuah referensi dianggap self-citation jika nama penulis paper dan nama author pada referensi memiliki kesamaan.  
+Referensi dengan Nomor 11 terindikasi self-citation.</t>
   </si>
   <si>
     <t>Tersitasi</t>
   </si>
   <si>
+    <t>Tidak Lengkap(*K)</t>
+  </si>
+  <si>
+    <t>Tidak Lengkap(*N)</t>
+  </si>
+  <si>
+    <t>Tidak Lengkap(*N *P)</t>
+  </si>
+  <si>
+    <t>Tidak Lengkap(*TT)</t>
+  </si>
+  <si>
+    <t>Tidak Lengkap(*V *N *T)</t>
+  </si>
+  <si>
     <t>Tidak Lengkap(*P)</t>
   </si>
   <si>
-    <t>Iya</t>
-  </si>
-  <si>
-    <t>Tidak Lengkap(*P *NJ)</t>
-  </si>
-  <si>
-    <t>Tidak Lengkap(*TT)</t>
-  </si>
-  <si>
-    <t>Tidak Lengkap(*K)</t>
-  </si>
-  <si>
-    <t>Tidak Lengkap(*N)</t>
-  </si>
-  <si>
-    <t>Referensi yang digunakan pada paper ini hanya menggunakan acuan primer sebesar 79.17%. Referensi dianggap beracuan primer ketika referensi tersebut berasal dari Jurnal, Conference, Buku, Thesis, dan Disertasi. 
-Referensi dengan Nomor 4 8 18 19 20 tidak beracuan primer.</t>
+    <t>Tidak Lengkap(*V *N)</t>
+  </si>
+  <si>
+    <t>Referensi yang digunakan pada paper ini menggunakan acuan primer sebesar 93.75%. Referensi dianggap beracuan primer ketika referensi tersebut berasal dari Jurnal, Conference, Buku, Thesis, dan Disertasi.  
+Referensi dengan Nomor 7 27 tidak beracuan primer.</t>
   </si>
   <si>
     <t>Format Lengkap</t>
   </si>
   <si>
-    <t>Terdapat 17 referensi yang memiliki format tidak lengkap. Referensi dianggap lengkap jika sudah mengikuti aturan referensi IEEE. Selain itu, referensi diluar Jurnal, Conference, Buku, Thesis, dan Disertasi juga akan dianggap tidak lengkap. 
-Referensi dengan Nomor 1 2 4 5 6 8 12 14 15 16 17 18 19 20 21 22 24 tidak berformat lengkap.</t>
+    <t>Terdapat 26 referensi yang memiliki format tidak lengkap. Referensi dianggap lengkap jika sudah mengikuti aturan referensi IEEE. Selain itu, referensi diluar Jurnal, Conference, Buku, Thesis, dan Disertasi juga akan dianggap tidak lengkap. 
+Referensi dengan Nomor 3 4 5 6 7 8 9 10 12 13 14 15 16 17 19 20 22 23 24 26 27 28 29 30 31 32 tidak berformat lengkap.</t>
   </si>
   <si>
     <t>Tersitasi Pada Naskah</t>
   </si>
   <si>
-    <t>Seluruh referensi telah disitasi pada naskah minimal 1 kali. Referensi dianggap tidak tersitasi pada naskah ketika referensi pada artikel ilmiah sama sekali tidak disitasi pada keseluruhan artikel.</t>
-  </si>
-  <si>
-    <t>Referensi yang digunakan pada pada paper ini masuk kedalam white list scopus sebesar 16.67%.
-Refernsi dengan Nomor 2 4 5 6 7 8 9 12 13 14 15 16 17 18 19 20 21 22 23 24 terindeks dalam white list scopus</t>
-  </si>
-  <si>
-    <t>Referensi yang digunakan pada pada paper ini masuk kedalam black list sebesar 8.33%. Data black list yang digunakan berasal dari bealls list. 
-Referensi dengan Nomor1 2 3 4 5 6 7 8 9 11 12 14 15 16 17 18 19 20 21 22 23 24terindeks dalam black list.</t>
+    <t>Terdapat 2 referensi yang tidak tersitasi pada naskah. Referensi dianggap tidak tersitasi pada naskah ketika referensi pada artikel ilmiah sama sekali tidak disitasi pada keseluruhan artikel. 
+Referensi dengan nomor 22 30 tidak disitasi pada naskah</t>
+  </si>
+  <si>
+    <t>Referensi yang digunakan pada pada paper ini masuk kedalam white list scopus sebesar 53.12%.
+Refernsi dengan Nomor 3 7 8 9 10 13 14 20 21 22 23 26 27 29 31 terindeks dalam white list scopus</t>
+  </si>
+  <si>
+    <t>Referensi yang digunakan pada pada paper ini masuk kedalam black list sebesar 0.00%. Data black list yang digunakan berasal dari bealls list. 
+Referensi dengan Nomor1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 25 26 27 28 29 30 31 32terindeks dalam black list.</t>
   </si>
 </sst>
 </file>
@@ -265,13 +303,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,8 +349,8 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -321,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -618,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -658,25 +696,25 @@
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J2" t="s">
@@ -687,25 +725,25 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J3" t="s">
@@ -716,25 +754,25 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J4" t="s">
@@ -745,25 +783,25 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>61</v>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
@@ -774,25 +812,25 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>62</v>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J6" t="s">
@@ -803,25 +841,25 @@
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>62</v>
+      <c r="B7" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J7" t="s">
@@ -832,25 +870,25 @@
       <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
+      <c r="B8" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -858,25 +896,25 @@
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>61</v>
+      <c r="B9" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="F9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -884,25 +922,25 @@
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="B10" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -910,26 +948,26 @@
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
+      <c r="B11" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -939,22 +977,22 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
-        <v>54</v>
+      <c r="C12" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -962,25 +1000,25 @@
       <c r="A13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>62</v>
+      <c r="B13" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -988,51 +1026,51 @@
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="B14" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>58</v>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1040,25 +1078,25 @@
       <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>62</v>
+      <c r="B16" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1066,25 +1104,25 @@
       <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>63</v>
+      <c r="B17" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1092,25 +1130,25 @@
       <c r="A18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>63</v>
+      <c r="B18" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>43</v>
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1118,25 +1156,25 @@
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>61</v>
+      <c r="B19" t="s">
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1144,25 +1182,25 @@
       <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
+      <c r="B20" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>45</v>
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1170,25 +1208,25 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1196,25 +1234,25 @@
       <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>63</v>
+      <c r="B22" t="s">
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1222,25 +1260,25 @@
       <c r="A23" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="3" t="s">
+      <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1248,25 +1286,25 @@
       <c r="A24" t="s">
         <v>41</v>
       </c>
-      <c r="B24" t="s">
-        <v>16</v>
+      <c r="B24" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1274,25 +1312,233 @@
       <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F25" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1320,10 +1566,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1331,31 +1577,31 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>67</v>
+      <c r="A8" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1363,7 +1609,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1371,7 +1617,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>